<commit_message>
Added another simulation for kmeans distances
</commit_message>
<xml_diff>
--- a/simulations.xlsx
+++ b/simulations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
   <si>
     <t>No</t>
   </si>
@@ -60,9 +60,6 @@
     <t>rgb</t>
   </si>
   <si>
-    <t>Initial experiments</t>
-  </si>
-  <si>
     <t>Test kmeans distance functions</t>
   </si>
   <si>
@@ -88,6 +85,15 @@
   </si>
   <si>
     <t>Manhattan</t>
+  </si>
+  <si>
+    <t>Experiments</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
   </si>
 </sst>
 </file>
@@ -456,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,12 +480,12 @@
     <col min="13" max="13" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -516,8 +522,17 @@
       <c r="L2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -555,7 +570,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -593,7 +608,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -631,7 +646,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -669,7 +684,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -707,7 +722,7 @@
         <v>0.55800000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -745,18 +760,62 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>200</v>
+      </c>
+      <c r="C9">
+        <v>200</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9">
+        <v>1600</v>
+      </c>
+      <c r="F9">
+        <v>1500</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <v>200</v>
+      </c>
+      <c r="K9">
+        <v>0.61</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="M9">
+        <v>0.24</v>
+      </c>
+      <c r="N9">
+        <v>0.38</v>
+      </c>
+      <c r="O9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L10" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -791,7 +850,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -827,24 +886,57 @@
       </c>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>200</v>
+      </c>
+      <c r="C15">
+        <v>200</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <v>1600</v>
+      </c>
+      <c r="F15">
+        <v>1500</v>
+      </c>
+      <c r="G15">
+        <v>100</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
+      <c r="J15">
+        <v>200</v>
+      </c>
+      <c r="K15">
+        <v>0.61</v>
+      </c>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -855,10 +947,10 @@
         <v>0.54600000000000004</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -869,10 +961,10 @@
         <v>0.67</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -883,10 +975,10 @@
         <v>0.6</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -897,10 +989,66 @@
         <v>0.54</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a bug with precision/recall calculations
</commit_message>
<xml_diff>
--- a/simulations.xlsx
+++ b/simulations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
   <si>
     <t>No</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Recall</t>
+  </si>
+  <si>
+    <t>Pos#/Neg#</t>
   </si>
 </sst>
 </file>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,14 +481,15 @@
     <col min="10" max="10" width="12.42578125" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
     <col min="13" max="13" width="18.5703125" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -531,8 +535,11 @@
       <c r="O2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -570,7 +577,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -608,7 +615,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -646,7 +653,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -684,7 +691,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -722,7 +729,7 @@
         <v>0.55800000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -760,7 +767,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -771,13 +778,13 @@
         <v>200</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9">
-        <v>1600</v>
+        <v>1900</v>
       </c>
       <c r="F9">
-        <v>1500</v>
+        <v>1800</v>
       </c>
       <c r="G9">
         <v>100</v>
@@ -795,235 +802,216 @@
         <v>0.61</v>
       </c>
       <c r="L9" s="1">
-        <v>0.65</v>
+        <v>0.63</v>
       </c>
       <c r="M9">
-        <v>0.24</v>
+        <v>0.75</v>
       </c>
       <c r="N9">
-        <v>0.38</v>
+        <v>0.62</v>
       </c>
       <c r="O9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="P9">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L10" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L12" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>0</v>
       </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>3</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E15" t="s">
         <v>4</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F15" t="s">
         <v>6</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G15" t="s">
         <v>5</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H15" t="s">
         <v>7</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I15" t="s">
         <v>8</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J15" t="s">
         <v>9</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14">
-        <v>200</v>
-      </c>
-      <c r="C14">
-        <v>200</v>
-      </c>
-      <c r="D14" t="s">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>200</v>
+      </c>
+      <c r="C16">
+        <v>200</v>
+      </c>
+      <c r="D16" t="s">
         <v>13</v>
       </c>
-      <c r="E14">
+      <c r="E16">
         <v>1000</v>
       </c>
-      <c r="F14">
+      <c r="F16">
         <v>900</v>
       </c>
-      <c r="G14">
+      <c r="G16">
         <v>100</v>
       </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
         <v>10</v>
       </c>
-      <c r="J14">
+      <c r="J16">
         <v>100</v>
       </c>
-      <c r="K14">
+      <c r="K16">
         <v>0.63</v>
       </c>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>2</v>
       </c>
-      <c r="B15">
-        <v>200</v>
-      </c>
-      <c r="C15">
-        <v>200</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="B17">
+        <v>200</v>
+      </c>
+      <c r="C17">
+        <v>200</v>
+      </c>
+      <c r="D17" t="s">
         <v>13</v>
       </c>
-      <c r="E15">
+      <c r="E17">
         <v>1600</v>
       </c>
-      <c r="F15">
+      <c r="F17">
         <v>1500</v>
       </c>
-      <c r="G15">
+      <c r="G17">
         <v>100</v>
       </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
         <v>10</v>
       </c>
-      <c r="J15">
-        <v>200</v>
-      </c>
-      <c r="K15">
+      <c r="J17">
+        <v>200</v>
+      </c>
+      <c r="K17">
         <v>0.61</v>
       </c>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>11</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>20</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2">
         <v>0.54600000000000004</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0.67</v>
-      </c>
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" s="1">
-        <v>0.6</v>
       </c>
       <c r="C20" t="s">
         <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" s="1">
-        <v>0.54</v>
+        <v>0.67</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" s="1">
-        <v>0.45</v>
+        <v>0.6</v>
       </c>
       <c r="C22" t="s">
         <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" s="1">
-        <v>0.64</v>
+        <v>0.54</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1034,20 +1022,48 @@
         <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
       <c r="B25" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1">
         <v>0.65</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C27" t="s">
         <v>22</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D27" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>